<commit_message>
May 25 with excel read and write
</commit_message>
<xml_diff>
--- a/testCase.xlsx
+++ b/testCase.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mdjal\Documents\GitHub\Expedia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1234163-1656-4A97-A8D8-1634AD336CA9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF271750-7707-4286-9004-708D66A3745D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{8362217D-B6F0-4CB0-B5D4-3FDAF29E380A}"/>
   </bookViews>
@@ -31,10 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
-  <si>
-    <t>seleniumtest2019@gmail.com</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>TestData</t>
   </si>
@@ -42,19 +39,25 @@
     <t>Name</t>
   </si>
   <si>
-    <t>email</t>
-  </si>
-  <si>
     <t>first name</t>
   </si>
   <si>
-    <t>Hassan</t>
-  </si>
-  <si>
     <t>Signup Text</t>
   </si>
   <si>
     <t>Sign Up</t>
+  </si>
+  <si>
+    <t>Jalil</t>
+  </si>
+  <si>
+    <t>destination</t>
+  </si>
+  <si>
+    <t>California</t>
+  </si>
+  <si>
+    <t>Get the Expedia App - text yourself a link</t>
   </si>
 </sst>
 </file>
@@ -111,7 +114,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -427,37 +430,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23A5487F-C98F-4F13-AF98-E667990D53DE}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="10.36328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
@@ -465,15 +468,20 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B5" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{DEC069F8-FF99-44C6-B71D-FDD6B0DB80F8}"/>
+    <hyperlink ref="B2" r:id="rId1" display="seleniumtest2019@gmail.com" xr:uid="{DEC069F8-FF99-44C6-B71D-FDD6B0DB80F8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId2"/>

</xml_diff>